<commit_message>
added code for memories
</commit_message>
<xml_diff>
--- a/purple_dreams.xlsx
+++ b/purple_dreams.xlsx
@@ -8,14 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/haripriyakrishnan/Downloads/Python/purple_dreams/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4035A0C8-4C47-AC41-8F98-6D6F5A028BD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0411086A-D543-8C46-8DB9-D87D577E5F4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5180" yWindow="1800" windowWidth="28040" windowHeight="17440" activeTab="2" xr2:uid="{52A6CF0C-9FDF-6A4B-B1CC-CBEE960F6C98}"/>
+    <workbookView xWindow="14540" yWindow="1800" windowWidth="18680" windowHeight="17440" xr2:uid="{52A6CF0C-9FDF-6A4B-B1CC-CBEE960F6C98}"/>
   </bookViews>
   <sheets>
-    <sheet name="Product" sheetId="2" r:id="rId1"/>
-    <sheet name="Discography" sheetId="1" r:id="rId2"/>
-    <sheet name="MusicVideo" sheetId="3" r:id="rId3"/>
+    <sheet name="Memory" sheetId="5" r:id="rId1"/>
+    <sheet name="Milestone" sheetId="4" r:id="rId2"/>
+    <sheet name="Discography" sheetId="1" r:id="rId3"/>
+    <sheet name="MusicVideo" sheetId="3" r:id="rId4"/>
+    <sheet name="Product" sheetId="2" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -37,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="666" uniqueCount="418">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="716" uniqueCount="441">
   <si>
     <t>Jungkook</t>
   </si>
@@ -927,9 +929,6 @@
     <t>https://www.youtube.com/watch?v=kkxdvBBQN_Y</t>
   </si>
   <si>
-    <t>V</t>
-  </si>
-  <si>
     <t>V ‘FRI(END)S’ Official MV</t>
   </si>
   <si>
@@ -1291,6 +1290,89 @@
   </si>
   <si>
     <t>video_name</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>Tae insta post 'Tiring Day'</t>
+  </si>
+  <si>
+    <t>Tae's Instagram Post</t>
+  </si>
+  <si>
+    <t>Tae In the Soop Friendcation</t>
+  </si>
+  <si>
+    <t>TaeKook</t>
+  </si>
+  <si>
+    <t>TaeKook Live</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Taehyung and Jungkook came on live along with Jin and Hobi. Tae mentioned about TaeKook's visit to Forture Teller </t>
+  </si>
+  <si>
+    <t>Tae about JK's Boxing</t>
+  </si>
+  <si>
+    <t>Tae comments on JK's boxing video</t>
+  </si>
+  <si>
+    <t>Jungkook Live on Weverse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jungkook posted on weverse and within a short span he came online. He sang so many songs for us along with Tae's Winter Ahead. </t>
+  </si>
+  <si>
+    <t>tae_tattoo.jpeg</t>
+  </si>
+  <si>
+    <t>be_fun.jpeg</t>
+  </si>
+  <si>
+    <t>jk_black.jpeg</t>
+  </si>
+  <si>
+    <t>jk_walk.jpeg</t>
+  </si>
+  <si>
+    <t>tk_inkigayo.jpeg</t>
+  </si>
+  <si>
+    <t>Asia Star No. 1</t>
+  </si>
+  <si>
+    <t>BTS V shines as a global presence, maintaining his title as 'The Most Influential Asian Star in the World' in 2024.
+V has solidified his position as the most notable star in Asia, proving his immense influence and popularity by ranking first in Asia on Instagram and Google Trends in 2024. In particular, V's star power and topicality stand out even more since this result came despite him being in the military. In an announcement of
+the most influential influencers by region and topic in 2024 by influencer analysis firm Hype Auditor, V was ranked 7th as 'The Most Influential Influencer in the World' and 'The Most Influential Influencer in the United States'. This is the highest ranking for an Asian star.
+The most influential star in the world on Instagram is Cristiano Ronaldo, with over 645 million followers. Pop star Taylor Swift, who came in second, was followed by Messi, Ariana Grande, Selena Gomez and Kendall Jenner, who took sixth place. In the UK, V ranked third after Taylor Swift and Ariana Grande, and is the most famous pop star excluding American pop stars. He ranked 4th in 'Most Influential Influencer in Music'. In addition, he ranked 8th and 2nd in Brazil and Indonesia, the centers of K-pop in South America and Asia, respectively, recording the highest ranking among Asian stars.
+V's topicality and popularity can also be confirmed in the 2024 Google Trends analysis. V ranked first as the most searched star among Asian celebrities in 2024, following 2021 and 2022.
+Virat Kohli, known as the greatest cricketer in history, ranked second, and Bollywood star and film producer Shahrukh Khan ranked third. V is also the K-pop star with the most searches on Google Trends from June 13, 2013, when BTS debuted, to December 2024. In 2024, he ranked 4th in the male pop star with the most searches on Google Trends, following Drake, Eminem, and Justin Bieber.
+V also has the most views among K-pop stars on Wikipedia. On Wikipedia, he ranked 7th in the male pop star most searched for worldwide this year, following Michael Jackson and Eminem. V is proving his global superstar status by ranking highest among Asian stars on Google, Wikipedia, and Instagram, which are included in the 'Top 5' website rankings (all industries).</t>
+  </si>
+  <si>
+    <t>tae_elegant.jpeg</t>
+  </si>
+  <si>
+    <t>New Record Music King</t>
+  </si>
+  <si>
+    <t>BTS' Jungkook continues his global presence by setting a new record as the first Asian solo artist to set a new record on the Billboard chart.
+According to the latest chart (dated December 21) released by Billboard, an American music media outlet, Jungkook's solo single "Seven" ranked 153rd on the "Global 200" chart.
+On the "Global (excl. US)" chart, it ranked 85th, successfully entering Billboard's two major charts once again and showing off his powerful music power.
+"Seven" has been on both the Billboard "Global 200" and "Global (excl. US)" charts for 74 consecutive weeks.With this, Jungkook has proven his global influence and fame as a solo artist by being the first and longest-serving Asian solo artist to be on both charts. Although
+"Seven" was released in July of last year, it has proven its popularity by captivating listeners around the world beyond its fandom by continuing to be active as a
+digital music source this year. "Seven" was included at number 28 on the "Top Tracks of 2024 Global" list, which is a year-end compilation of the most streamed (played) songs worldwide this year, revealed by Spotify, the world's largest music streaming platform. It also surpassed 2.1 billion streams (before filtering) in 518 days on Spotify, the "shortest" period for an Asian singer.</t>
+  </si>
+  <si>
+    <t>jungkook_pop.jpeg</t>
   </si>
 </sst>
 </file>
@@ -1363,7 +1445,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1372,6 +1454,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1686,50 +1772,156 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADE86AF9-D9C6-C14D-B882-6BAE66AC5796}">
-  <dimension ref="A1:C3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FC3AAAE-FAA3-9841-A3E8-32EF7D55B7D2}">
+  <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.1640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="80.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="C1" s="5" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B2">
-        <v>1.99</v>
+      <c r="E1" s="1" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="8">
+        <v>43838</v>
+      </c>
+      <c r="B2" t="s">
+        <v>23</v>
       </c>
       <c r="C2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>57</v>
-      </c>
-      <c r="B3">
-        <v>0.99</v>
+        <v>421</v>
+      </c>
+      <c r="D2" t="s">
+        <v>430</v>
+      </c>
+      <c r="E2" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="8">
+        <v>43839</v>
+      </c>
+      <c r="B3" t="s">
+        <v>23</v>
       </c>
       <c r="C3" t="s">
-        <v>58</v>
+        <v>422</v>
+      </c>
+      <c r="D3" t="s">
+        <v>431</v>
+      </c>
+      <c r="E3" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="8">
+        <v>43856</v>
+      </c>
+      <c r="B4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" t="s">
+        <v>426</v>
+      </c>
+      <c r="D4" t="s">
+        <v>432</v>
+      </c>
+      <c r="E4" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="8">
+        <v>43896</v>
+      </c>
+      <c r="B5" t="s">
+        <v>423</v>
+      </c>
+      <c r="C5" t="s">
+        <v>424</v>
+      </c>
+      <c r="D5" t="s">
+        <v>434</v>
+      </c>
+      <c r="E5" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="8">
+        <v>45644</v>
+      </c>
+      <c r="B6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" t="s">
+        <v>428</v>
+      </c>
+      <c r="D6" t="s">
+        <v>433</v>
+      </c>
+      <c r="E6" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="409.5" x14ac:dyDescent="0.2">
+      <c r="A7" s="8">
+        <v>45648</v>
+      </c>
+      <c r="B7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" t="s">
+        <v>435</v>
+      </c>
+      <c r="D7" t="s">
+        <v>437</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="356" x14ac:dyDescent="0.2">
+      <c r="A8" s="8">
+        <v>45648</v>
+      </c>
+      <c r="B8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" t="s">
+        <v>438</v>
+      </c>
+      <c r="D8" t="s">
+        <v>440</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>439</v>
       </c>
     </row>
   </sheetData>
@@ -1738,12 +1930,100 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FF545AA-6E8A-4041-8C85-5E93936F26FB}">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="9.1640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="8">
+        <v>43839</v>
+      </c>
+      <c r="B2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" t="s">
+        <v>422</v>
+      </c>
+      <c r="D2" t="s">
+        <v>431</v>
+      </c>
+      <c r="E2" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="8">
+        <v>43896</v>
+      </c>
+      <c r="B3" t="s">
+        <v>423</v>
+      </c>
+      <c r="C3" t="s">
+        <v>424</v>
+      </c>
+      <c r="D3" t="s">
+        <v>434</v>
+      </c>
+      <c r="E3" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="8">
+        <v>45644</v>
+      </c>
+      <c r="B4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" t="s">
+        <v>428</v>
+      </c>
+      <c r="D4" t="s">
+        <v>433</v>
+      </c>
+      <c r="E4" t="s">
+        <v>429</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E3C3D97-69CD-0B46-9892-9CF02B5710A8}">
   <dimension ref="A1:N931"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -17075,11 +17355,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B981EFC-1AD7-EC4B-9347-256C8C05A87B}">
   <dimension ref="A1:C177"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -17093,7 +17373,7 @@
         <v>47</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>70</v>
@@ -18355,684 +18635,684 @@
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A116" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B116" s="2" t="s">
         <v>296</v>
       </c>
-      <c r="B116" s="2" t="s">
+      <c r="C116" s="7" t="s">
         <v>297</v>
-      </c>
-      <c r="C116" s="7" t="s">
-        <v>298</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A117" s="2" t="s">
-        <v>296</v>
+        <v>23</v>
       </c>
       <c r="B117" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="C117" s="7" t="s">
         <v>299</v>
-      </c>
-      <c r="C117" s="7" t="s">
-        <v>300</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A118" s="2" t="s">
-        <v>296</v>
+        <v>23</v>
       </c>
       <c r="B118" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="C118" s="7" t="s">
         <v>301</v>
-      </c>
-      <c r="C118" s="7" t="s">
-        <v>302</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A119" s="2" t="s">
-        <v>296</v>
+        <v>23</v>
       </c>
       <c r="B119" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="C119" s="7" t="s">
         <v>303</v>
-      </c>
-      <c r="C119" s="7" t="s">
-        <v>304</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A120" s="2" t="s">
-        <v>296</v>
+        <v>23</v>
       </c>
       <c r="B120" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="C120" s="7" t="s">
         <v>305</v>
-      </c>
-      <c r="C120" s="7" t="s">
-        <v>306</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A121" s="2" t="s">
-        <v>296</v>
+        <v>23</v>
       </c>
       <c r="B121" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="C121" s="7" t="s">
         <v>307</v>
-      </c>
-      <c r="C121" s="7" t="s">
-        <v>308</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A122" s="2" t="s">
-        <v>296</v>
+        <v>23</v>
       </c>
       <c r="B122" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="C122" s="7" t="s">
         <v>309</v>
-      </c>
-      <c r="C122" s="7" t="s">
-        <v>310</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A123" s="2" t="s">
-        <v>296</v>
+        <v>23</v>
       </c>
       <c r="B123" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="C123" s="7" t="s">
         <v>311</v>
-      </c>
-      <c r="C123" s="7" t="s">
-        <v>312</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A124" s="2" t="s">
-        <v>296</v>
+        <v>23</v>
       </c>
       <c r="B124" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="C124" s="7" t="s">
         <v>313</v>
-      </c>
-      <c r="C124" s="7" t="s">
-        <v>314</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A125" s="2" t="s">
-        <v>296</v>
+        <v>23</v>
       </c>
       <c r="B125" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="C125" s="7" t="s">
         <v>315</v>
-      </c>
-      <c r="C125" s="7" t="s">
-        <v>316</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A126" s="2" t="s">
-        <v>296</v>
+        <v>23</v>
       </c>
       <c r="B126" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="C126" s="7" t="s">
         <v>317</v>
-      </c>
-      <c r="C126" s="7" t="s">
-        <v>318</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A127" s="2" t="s">
-        <v>296</v>
+        <v>23</v>
       </c>
       <c r="B127" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="C127" s="7" t="s">
         <v>319</v>
-      </c>
-      <c r="C127" s="7" t="s">
-        <v>320</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A128" s="2" t="s">
-        <v>296</v>
+        <v>23</v>
       </c>
       <c r="B128" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="C128" s="7" t="s">
         <v>321</v>
-      </c>
-      <c r="C128" s="7" t="s">
-        <v>322</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A129" s="2" t="s">
-        <v>296</v>
+        <v>23</v>
       </c>
       <c r="B129" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="C129" s="7" t="s">
         <v>323</v>
-      </c>
-      <c r="C129" s="7" t="s">
-        <v>324</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A130" s="2" t="s">
-        <v>296</v>
+        <v>23</v>
       </c>
       <c r="B130" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="C130" s="7" t="s">
         <v>325</v>
-      </c>
-      <c r="C130" s="7" t="s">
-        <v>326</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A131" s="2" t="s">
-        <v>296</v>
+        <v>23</v>
       </c>
       <c r="B131" s="2" t="s">
         <v>37</v>
       </c>
       <c r="C131" s="7" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A132" s="2" t="s">
-        <v>296</v>
+        <v>23</v>
       </c>
       <c r="B132" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="C132" s="7" t="s">
         <v>328</v>
-      </c>
-      <c r="C132" s="7" t="s">
-        <v>329</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A133" s="2" t="s">
-        <v>296</v>
+        <v>23</v>
       </c>
       <c r="B133" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="C133" s="7" t="s">
         <v>330</v>
-      </c>
-      <c r="C133" s="7" t="s">
-        <v>331</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A134" s="2" t="s">
-        <v>296</v>
+        <v>23</v>
       </c>
       <c r="B134" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="C134" s="7" t="s">
         <v>332</v>
-      </c>
-      <c r="C134" s="7" t="s">
-        <v>333</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A135" s="2" t="s">
-        <v>296</v>
+        <v>23</v>
       </c>
       <c r="B135" s="2" t="s">
         <v>28</v>
       </c>
       <c r="C135" s="7" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A136" s="2" t="s">
-        <v>296</v>
+        <v>23</v>
       </c>
       <c r="B136" s="2" t="s">
+        <v>334</v>
+      </c>
+      <c r="C136" s="7" t="s">
         <v>335</v>
-      </c>
-      <c r="C136" s="7" t="s">
-        <v>336</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A137" s="2" t="s">
-        <v>296</v>
+        <v>23</v>
       </c>
       <c r="B137" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C137" s="7" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A138" s="2" t="s">
-        <v>296</v>
+        <v>23</v>
       </c>
       <c r="B138" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C138" s="7" t="s">
         <v>338</v>
-      </c>
-      <c r="C138" s="7" t="s">
-        <v>339</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A139" s="2" t="s">
-        <v>296</v>
+        <v>23</v>
       </c>
       <c r="B139" s="2" t="s">
+        <v>339</v>
+      </c>
+      <c r="C139" s="7" t="s">
         <v>340</v>
-      </c>
-      <c r="C139" s="7" t="s">
-        <v>341</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A140" s="2" t="s">
-        <v>296</v>
+        <v>23</v>
       </c>
       <c r="B140" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="C140" s="7" t="s">
         <v>342</v>
-      </c>
-      <c r="C140" s="7" t="s">
-        <v>343</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A141" s="2" t="s">
-        <v>296</v>
+        <v>23</v>
       </c>
       <c r="B141" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="C141" s="7" t="s">
         <v>344</v>
-      </c>
-      <c r="C141" s="7" t="s">
-        <v>345</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A142" s="2" t="s">
-        <v>296</v>
+        <v>23</v>
       </c>
       <c r="B142" s="2" t="s">
+        <v>345</v>
+      </c>
+      <c r="C142" s="7" t="s">
         <v>346</v>
-      </c>
-      <c r="C142" s="7" t="s">
-        <v>347</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A143" s="2" t="s">
-        <v>296</v>
+        <v>23</v>
       </c>
       <c r="B143" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="C143" s="7" t="s">
         <v>348</v>
-      </c>
-      <c r="C143" s="7" t="s">
-        <v>349</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A144" s="2" t="s">
-        <v>296</v>
+        <v>23</v>
       </c>
       <c r="B144" s="2" t="s">
+        <v>349</v>
+      </c>
+      <c r="C144" s="7" t="s">
         <v>350</v>
-      </c>
-      <c r="C144" s="7" t="s">
-        <v>351</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A145" s="2" t="s">
-        <v>296</v>
+        <v>23</v>
       </c>
       <c r="B145" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="C145" s="7" t="s">
         <v>352</v>
-      </c>
-      <c r="C145" s="7" t="s">
-        <v>353</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A146" s="2" t="s">
-        <v>296</v>
+        <v>23</v>
       </c>
       <c r="B146" s="2" t="s">
+        <v>353</v>
+      </c>
+      <c r="C146" s="7" t="s">
         <v>354</v>
-      </c>
-      <c r="C146" s="7" t="s">
-        <v>355</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A147" s="2" t="s">
-        <v>296</v>
+        <v>23</v>
       </c>
       <c r="B147" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="C147" s="7" t="s">
         <v>356</v>
-      </c>
-      <c r="C147" s="7" t="s">
-        <v>357</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A148" s="2" t="s">
-        <v>296</v>
+        <v>23</v>
       </c>
       <c r="B148" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="C148" s="7" t="s">
         <v>358</v>
-      </c>
-      <c r="C148" s="7" t="s">
-        <v>359</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A149" s="2" t="s">
-        <v>296</v>
+        <v>23</v>
       </c>
       <c r="B149" s="2" t="s">
+        <v>359</v>
+      </c>
+      <c r="C149" s="7" t="s">
         <v>360</v>
-      </c>
-      <c r="C149" s="7" t="s">
-        <v>361</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A150" s="2" t="s">
-        <v>296</v>
+        <v>23</v>
       </c>
       <c r="B150" s="2" t="s">
+        <v>361</v>
+      </c>
+      <c r="C150" s="7" t="s">
         <v>362</v>
-      </c>
-      <c r="C150" s="7" t="s">
-        <v>363</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A151" s="2" t="s">
-        <v>296</v>
+        <v>23</v>
       </c>
       <c r="B151" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="C151" s="7" t="s">
         <v>364</v>
-      </c>
-      <c r="C151" s="7" t="s">
-        <v>365</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A152" s="2" t="s">
-        <v>296</v>
+        <v>23</v>
       </c>
       <c r="B152" s="2" t="s">
+        <v>365</v>
+      </c>
+      <c r="C152" s="7" t="s">
         <v>366</v>
-      </c>
-      <c r="C152" s="7" t="s">
-        <v>367</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A153" s="2" t="s">
-        <v>296</v>
+        <v>23</v>
       </c>
       <c r="B153" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="C153" s="7" t="s">
         <v>368</v>
-      </c>
-      <c r="C153" s="7" t="s">
-        <v>369</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A154" s="2" t="s">
-        <v>296</v>
+        <v>23</v>
       </c>
       <c r="B154" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="C154" s="7" t="s">
         <v>370</v>
-      </c>
-      <c r="C154" s="7" t="s">
-        <v>371</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A155" s="2" t="s">
-        <v>296</v>
+        <v>23</v>
       </c>
       <c r="B155" s="2" t="s">
+        <v>371</v>
+      </c>
+      <c r="C155" s="7" t="s">
         <v>372</v>
-      </c>
-      <c r="C155" s="7" t="s">
-        <v>373</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A156" s="2" t="s">
-        <v>296</v>
+        <v>23</v>
       </c>
       <c r="B156" s="2" t="s">
+        <v>373</v>
+      </c>
+      <c r="C156" s="7" t="s">
         <v>374</v>
-      </c>
-      <c r="C156" s="7" t="s">
-        <v>375</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A157" s="2" t="s">
-        <v>296</v>
+        <v>23</v>
       </c>
       <c r="B157" s="2" t="s">
+        <v>375</v>
+      </c>
+      <c r="C157" s="7" t="s">
         <v>376</v>
-      </c>
-      <c r="C157" s="7" t="s">
-        <v>377</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A158" s="2" t="s">
-        <v>296</v>
+        <v>23</v>
       </c>
       <c r="B158" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="C158" s="7" t="s">
         <v>378</v>
-      </c>
-      <c r="C158" s="7" t="s">
-        <v>379</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A159" s="2" t="s">
-        <v>296</v>
+        <v>23</v>
       </c>
       <c r="B159" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="C159" s="7" t="s">
         <v>380</v>
-      </c>
-      <c r="C159" s="7" t="s">
-        <v>381</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A160" s="2" t="s">
-        <v>296</v>
+        <v>23</v>
       </c>
       <c r="B160" s="2" t="s">
+        <v>381</v>
+      </c>
+      <c r="C160" s="7" t="s">
         <v>382</v>
-      </c>
-      <c r="C160" s="7" t="s">
-        <v>383</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A161" s="2" t="s">
-        <v>296</v>
+        <v>23</v>
       </c>
       <c r="B161" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="C161" s="7" t="s">
         <v>384</v>
-      </c>
-      <c r="C161" s="7" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A162" s="2" t="s">
-        <v>296</v>
+        <v>23</v>
       </c>
       <c r="B162" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="C162" s="7" t="s">
         <v>386</v>
-      </c>
-      <c r="C162" s="7" t="s">
-        <v>387</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A163" s="2" t="s">
-        <v>296</v>
+        <v>23</v>
       </c>
       <c r="B163" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="C163" s="7" t="s">
         <v>388</v>
-      </c>
-      <c r="C163" s="7" t="s">
-        <v>389</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A164" s="2" t="s">
-        <v>296</v>
+        <v>23</v>
       </c>
       <c r="B164" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="C164" s="7" t="s">
         <v>390</v>
-      </c>
-      <c r="C164" s="7" t="s">
-        <v>391</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A165" s="2" t="s">
-        <v>296</v>
+        <v>23</v>
       </c>
       <c r="B165" s="2" t="s">
+        <v>391</v>
+      </c>
+      <c r="C165" s="7" t="s">
         <v>392</v>
-      </c>
-      <c r="C165" s="7" t="s">
-        <v>393</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A166" s="2" t="s">
-        <v>296</v>
+        <v>23</v>
       </c>
       <c r="B166" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="C166" s="7" t="s">
         <v>394</v>
-      </c>
-      <c r="C166" s="7" t="s">
-        <v>395</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A167" s="2" t="s">
-        <v>296</v>
+        <v>23</v>
       </c>
       <c r="B167" s="2" t="s">
+        <v>395</v>
+      </c>
+      <c r="C167" s="7" t="s">
         <v>396</v>
-      </c>
-      <c r="C167" s="7" t="s">
-        <v>397</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A168" s="2" t="s">
-        <v>296</v>
+        <v>23</v>
       </c>
       <c r="B168" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="C168" s="7" t="s">
         <v>398</v>
-      </c>
-      <c r="C168" s="7" t="s">
-        <v>399</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A169" s="2" t="s">
-        <v>296</v>
+        <v>23</v>
       </c>
       <c r="B169" s="2" t="s">
+        <v>399</v>
+      </c>
+      <c r="C169" s="6" t="s">
         <v>400</v>
-      </c>
-      <c r="C169" s="6" t="s">
-        <v>401</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A170" s="2" t="s">
-        <v>296</v>
+        <v>23</v>
       </c>
       <c r="B170" s="2" t="s">
+        <v>401</v>
+      </c>
+      <c r="C170" s="6" t="s">
         <v>402</v>
-      </c>
-      <c r="C170" s="6" t="s">
-        <v>403</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A171" s="2" t="s">
-        <v>296</v>
+        <v>23</v>
       </c>
       <c r="B171" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="C171" s="6" t="s">
         <v>404</v>
-      </c>
-      <c r="C171" s="6" t="s">
-        <v>405</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A172" s="2" t="s">
-        <v>296</v>
+        <v>23</v>
       </c>
       <c r="B172" s="2" t="s">
+        <v>405</v>
+      </c>
+      <c r="C172" s="6" t="s">
         <v>406</v>
-      </c>
-      <c r="C172" s="6" t="s">
-        <v>407</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A173" s="2" t="s">
-        <v>296</v>
+        <v>23</v>
       </c>
       <c r="B173" s="2" t="s">
         <v>60</v>
       </c>
       <c r="C173" s="6" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A174" s="2" t="s">
-        <v>296</v>
+        <v>23</v>
       </c>
       <c r="B174" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="C174" s="6" t="s">
         <v>409</v>
-      </c>
-      <c r="C174" s="6" t="s">
-        <v>410</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A175" s="2" t="s">
-        <v>296</v>
+        <v>23</v>
       </c>
       <c r="B175" s="2" t="s">
+        <v>410</v>
+      </c>
+      <c r="C175" s="7" t="s">
         <v>411</v>
-      </c>
-      <c r="C175" s="7" t="s">
-        <v>412</v>
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A176" s="2" t="s">
-        <v>296</v>
+        <v>23</v>
       </c>
       <c r="B176" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="C176" s="7" t="s">
         <v>413</v>
-      </c>
-      <c r="C176" s="7" t="s">
-        <v>414</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A177" s="2" t="s">
-        <v>296</v>
+        <v>23</v>
       </c>
       <c r="B177" s="2" t="s">
+        <v>414</v>
+      </c>
+      <c r="C177" s="7" t="s">
         <v>415</v>
-      </c>
-      <c r="C177" s="7" t="s">
-        <v>416</v>
       </c>
     </row>
   </sheetData>
@@ -19210,4 +19490,56 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADE86AF9-D9C6-C14D-B882-6BAE66AC5796}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2">
+        <v>1.99</v>
+      </c>
+      <c r="C2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B3">
+        <v>0.99</v>
+      </c>
+      <c r="C3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
updated styles for memories
</commit_message>
<xml_diff>
--- a/purple_dreams.xlsx
+++ b/purple_dreams.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/haripriyakrishnan/Downloads/Python/purple_dreams/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0411086A-D543-8C46-8DB9-D87D577E5F4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B3E8158-030A-E644-A881-5002ADA1EB4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14540" yWindow="1800" windowWidth="18680" windowHeight="17440" xr2:uid="{52A6CF0C-9FDF-6A4B-B1CC-CBEE960F6C98}"/>
   </bookViews>
@@ -1773,10 +1773,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FC3AAAE-FAA3-9841-A3E8-32EF7D55B7D2}">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1890,40 +1890,6 @@
         <v>429</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="409.5" x14ac:dyDescent="0.2">
-      <c r="A7" s="8">
-        <v>45648</v>
-      </c>
-      <c r="B7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" t="s">
-        <v>435</v>
-      </c>
-      <c r="D7" t="s">
-        <v>437</v>
-      </c>
-      <c r="E7" s="9" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="356" x14ac:dyDescent="0.2">
-      <c r="A8" s="8">
-        <v>45648</v>
-      </c>
-      <c r="B8" t="s">
-        <v>0</v>
-      </c>
-      <c r="C8" t="s">
-        <v>438</v>
-      </c>
-      <c r="D8" t="s">
-        <v>440</v>
-      </c>
-      <c r="E8" s="9" t="s">
-        <v>439</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1931,10 +1897,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FF545AA-6E8A-4041-8C85-5E93936F26FB}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1943,7 +1909,7 @@
     <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="71.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
@@ -2012,6 +1978,40 @@
       </c>
       <c r="E4" t="s">
         <v>429</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A5" s="8">
+        <v>45648</v>
+      </c>
+      <c r="B5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" t="s">
+        <v>435</v>
+      </c>
+      <c r="D5" t="s">
+        <v>437</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="388" x14ac:dyDescent="0.2">
+      <c r="A6" s="8">
+        <v>45648</v>
+      </c>
+      <c r="B6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" t="s">
+        <v>438</v>
+      </c>
+      <c r="D6" t="s">
+        <v>440</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>439</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added code for Upcoming events
</commit_message>
<xml_diff>
--- a/purple_dreams.xlsx
+++ b/purple_dreams.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/haripriyakrishnan/Downloads/Python/purple_dreams/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2B91609-D657-C542-B5D7-83F28E1C73D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFD52128-8AB4-B34A-B960-D1115E70DBDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14540" yWindow="1800" windowWidth="18680" windowHeight="17440" xr2:uid="{52A6CF0C-9FDF-6A4B-B1CC-CBEE960F6C98}"/>
   </bookViews>
   <sheets>
-    <sheet name="Memory" sheetId="5" r:id="rId1"/>
-    <sheet name="Milestone" sheetId="4" r:id="rId2"/>
-    <sheet name="Discography" sheetId="1" r:id="rId3"/>
-    <sheet name="MusicVideo" sheetId="3" r:id="rId4"/>
-    <sheet name="Product" sheetId="2" r:id="rId5"/>
+    <sheet name="Upcoming" sheetId="6" r:id="rId1"/>
+    <sheet name="Memory" sheetId="5" r:id="rId2"/>
+    <sheet name="Milestone" sheetId="4" r:id="rId3"/>
+    <sheet name="Discography" sheetId="1" r:id="rId4"/>
+    <sheet name="MusicVideo" sheetId="3" r:id="rId5"/>
+    <sheet name="Product" sheetId="2" r:id="rId6"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="716" uniqueCount="441">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="733" uniqueCount="448">
   <si>
     <t>Jungkook</t>
   </si>
@@ -1373,6 +1374,27 @@
   </si>
   <si>
     <t>jungkook_pop.jpeg</t>
+  </si>
+  <si>
+    <t>Taehyung Chapter 2</t>
+  </si>
+  <si>
+    <t>Jungkook Chapter 2</t>
+  </si>
+  <si>
+    <t>TaeKook Subunit</t>
+  </si>
+  <si>
+    <t>tk_purple.jpeg</t>
+  </si>
+  <si>
+    <t>Taehyung and Jungkook coming together to give us a subunit song for TeteKooFM. Join TeteKooFM and enjoy the song.</t>
+  </si>
+  <si>
+    <t>Jungkook is releasing his second solo Album</t>
+  </si>
+  <si>
+    <t>Taehyung is releasing his second solo Album</t>
   </si>
 </sst>
 </file>
@@ -1772,11 +1794,99 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B9BFF86-0677-E440-B359-1099C3CCEA5D}">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:E1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="8">
+        <v>45666</v>
+      </c>
+      <c r="B2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" t="s">
+        <v>441</v>
+      </c>
+      <c r="D2" t="s">
+        <v>437</v>
+      </c>
+      <c r="E2" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="8">
+        <v>45683</v>
+      </c>
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>442</v>
+      </c>
+      <c r="D3" t="s">
+        <v>440</v>
+      </c>
+      <c r="E3" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="8">
+        <v>45752</v>
+      </c>
+      <c r="B4" t="s">
+        <v>423</v>
+      </c>
+      <c r="C4" t="s">
+        <v>443</v>
+      </c>
+      <c r="D4" t="s">
+        <v>444</v>
+      </c>
+      <c r="E4" t="s">
+        <v>445</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FC3AAAE-FAA3-9841-A3E8-32EF7D55B7D2}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1895,7 +2005,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FF545AA-6E8A-4041-8C85-5E93936F26FB}">
   <dimension ref="A1:E6"/>
   <sheetViews>
@@ -2019,7 +2129,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E3C3D97-69CD-0B46-9892-9CF02B5710A8}">
   <dimension ref="A1:N931"/>
   <sheetViews>
@@ -17355,7 +17465,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B981EFC-1AD7-EC4B-9347-256C8C05A87B}">
   <dimension ref="A1:C177"/>
   <sheetViews>
@@ -19492,7 +19602,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADE86AF9-D9C6-C14D-B882-6BAE66AC5796}">
   <dimension ref="A1:C3"/>
   <sheetViews>

</xml_diff>